<commit_message>
Updated for SharePoint Sites
</commit_message>
<xml_diff>
--- a/LabSources/365DataEnvironment.xlsx
+++ b/LabSources/365DataEnvironment.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubDell\365AutomatedLab\LabSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9207FE33-8A15-410C-9829-3DC42B7B1EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CD58EB-E763-4855-B07D-A5DD53B988A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="3555" windowWidth="13365" windowHeight="12645" activeTab="3" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
+    <workbookView xWindow="26610" yWindow="2640" windowWidth="13500" windowHeight="12825" activeTab="4" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Groups" sheetId="2" r:id="rId2"/>
     <sheet name="NY-IT" sheetId="3" r:id="rId3"/>
     <sheet name="Teams" sheetId="4" r:id="rId4"/>
+    <sheet name="Sites" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="261">
   <si>
     <t>FirstName</t>
   </si>
@@ -753,13 +754,82 @@
   </si>
   <si>
     <t>Client Meetings</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>SiteType</t>
+  </si>
+  <si>
+    <t>EHS#1</t>
+  </si>
+  <si>
+    <t>TeamSite</t>
+  </si>
+  <si>
+    <t>Blog25</t>
+  </si>
+  <si>
+    <t>BLOG#0</t>
+  </si>
+  <si>
+    <t>CommunicationSite</t>
+  </si>
+  <si>
+    <t>Project25</t>
+  </si>
+  <si>
+    <t>PROJECTSITE#0</t>
+  </si>
+  <si>
+    <t>TeamSiteWithoutMicrosoft365Group</t>
+  </si>
+  <si>
+    <t>Community25</t>
+  </si>
+  <si>
+    <t>COMMUNITY#0</t>
+  </si>
+  <si>
+    <t>TestTeam25</t>
+  </si>
+  <si>
+    <t>TestCommunication25</t>
+  </si>
+  <si>
+    <t>TestProjectteamwithout36255</t>
+  </si>
+  <si>
+    <t>TestCommunityTeam25</t>
+  </si>
+  <si>
+    <t>Test Team Site 25</t>
+  </si>
+  <si>
+    <t>Test Blog 25</t>
+  </si>
+  <si>
+    <t>Project Test project site 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Community Site 25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,6 +843,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -795,9 +871,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2576,7 +2660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEBB1DA-38E9-45D2-BDE5-11FE78334DE3}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2647,4 +2731,127 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B2B338-EC44-4B0B-9532-D06A3843D7DA}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="4">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="4">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Fields in 365DataEnvironment for new features
</commit_message>
<xml_diff>
--- a/LabSources/365DataEnvironment.xlsx
+++ b/LabSources/365DataEnvironment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubDell\365AutomatedLab\LabSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA9FA72-2AE5-4464-9104-41D72992FF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A6B854-CCBC-446A-8C76-41B9C0DAFB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23130" yWindow="1890" windowWidth="22185" windowHeight="13065" activeTab="1" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
+    <workbookView xWindow="1605" yWindow="17355" windowWidth="15030" windowHeight="13065" activeTab="3" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="271">
   <si>
     <t>FirstName</t>
   </si>
@@ -835,6 +835,24 @@
   </si>
   <si>
     <t>Confidential</t>
+  </si>
+  <si>
+    <t>TeamType</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Channel1Type</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>Channel2Type</t>
   </si>
 </sst>
 </file>
@@ -2248,7 +2266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6396F3-6D7B-46A0-9EAC-B306C37237B1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2670,21 +2688,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEBB1DA-38E9-45D2-BDE5-11FE78334DE3}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>220</v>
       </c>
@@ -2692,13 +2712,22 @@
         <v>221</v>
       </c>
       <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
         <v>222</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>224</v>
       </c>
@@ -2706,13 +2735,22 @@
         <v>225</v>
       </c>
       <c r="C2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
         <v>226</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -2720,13 +2758,22 @@
         <v>250</v>
       </c>
       <c r="C3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" t="s">
         <v>251</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>269</v>
+      </c>
+      <c r="F3" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>253</v>
       </c>
@@ -2734,13 +2781,22 @@
         <v>254</v>
       </c>
       <c r="C4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" t="s">
         <v>255</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F4" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>261</v>
       </c>
@@ -2748,10 +2804,19 @@
         <v>262</v>
       </c>
       <c r="C5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" t="s">
         <v>263</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F5" t="s">
         <v>264</v>
+      </c>
+      <c r="G5" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new features for Adding Teams and Channels
</commit_message>
<xml_diff>
--- a/LabSources/365DataEnvironment.xlsx
+++ b/LabSources/365DataEnvironment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubDell\365AutomatedLab\LabSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A6B854-CCBC-446A-8C76-41B9C0DAFB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D62A3E0-CE27-4AE6-AFFC-A26BE94B81FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="17355" windowWidth="15030" windowHeight="13065" activeTab="3" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
+    <workbookView xWindow="19710" yWindow="1350" windowWidth="22740" windowHeight="13590" activeTab="3" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="281">
   <si>
     <t>FirstName</t>
   </si>
@@ -853,6 +853,36 @@
   </si>
   <si>
     <t>Channel2Type</t>
+  </si>
+  <si>
+    <t>Channel1Description</t>
+  </si>
+  <si>
+    <t>Channel for all Marketing Campaigns</t>
+  </si>
+  <si>
+    <t>Channel2Description</t>
+  </si>
+  <si>
+    <t>Channel for Brainstorming</t>
+  </si>
+  <si>
+    <t>Channel for all agreements</t>
+  </si>
+  <si>
+    <t>A private channel for confidential information</t>
+  </si>
+  <si>
+    <t>A private channel for projects</t>
+  </si>
+  <si>
+    <t>Channel for all Incidents</t>
+  </si>
+  <si>
+    <t>Channel for all contracts</t>
+  </si>
+  <si>
+    <t>Channel for all onboarding</t>
   </si>
 </sst>
 </file>
@@ -929,9 +959,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -969,7 +999,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1075,7 +1105,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1217,7 +1247,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2688,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEBB1DA-38E9-45D2-BDE5-11FE78334DE3}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,11 +2730,13 @@
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>220</v>
       </c>
@@ -2718,16 +2750,22 @@
         <v>222</v>
       </c>
       <c r="E1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" t="s">
         <v>267</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>223</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>224</v>
       </c>
@@ -2741,16 +2779,22 @@
         <v>226</v>
       </c>
       <c r="E2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" t="s">
         <v>268</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>227</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>274</v>
+      </c>
+      <c r="I2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -2764,16 +2808,22 @@
         <v>251</v>
       </c>
       <c r="E3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F3" t="s">
         <v>269</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>252</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>277</v>
+      </c>
+      <c r="I3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>253</v>
       </c>
@@ -2787,16 +2837,22 @@
         <v>255</v>
       </c>
       <c r="E4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4" t="s">
         <v>269</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>256</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>261</v>
       </c>
@@ -2810,12 +2866,18 @@
         <v>263</v>
       </c>
       <c r="E5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F5" t="s">
         <v>269</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>264</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I5" t="s">
         <v>269</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated columns to match new parameters
</commit_message>
<xml_diff>
--- a/LabSources/365DataEnvironment.xlsx
+++ b/LabSources/365DataEnvironment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubDell\365AutomatedLab\LabSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive - Clate\Documents\GitHub\Testing\365\New User\Adding Params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC4822D-C922-4A83-A490-89262768CB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B93F71A-7B07-41BE-BD9E-72CD58BE1EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21195" yWindow="3015" windowWidth="23085" windowHeight="13065" activeTab="1" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
+    <workbookView xWindow="4815" yWindow="655" windowWidth="9110" windowHeight="9020" xr2:uid="{D69C5377-2701-4485-B57B-1A8C43364DD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="314">
   <si>
     <t>FirstName</t>
   </si>
@@ -886,13 +886,112 @@
   </si>
   <si>
     <t>ManagedBy</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>EmployeeHireDate</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>EmployeeType</t>
+  </si>
+  <si>
+    <t>Testing Comp</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Contractor</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>FaxNumber</t>
+  </si>
+  <si>
+    <t>212-555-7777</t>
+  </si>
+  <si>
+    <t>212-555-7778</t>
+  </si>
+  <si>
+    <t>212-555-7779</t>
+  </si>
+  <si>
+    <t>212-555-7780</t>
+  </si>
+  <si>
+    <t>212-555-7781</t>
+  </si>
+  <si>
+    <t>212-555-7782</t>
+  </si>
+  <si>
+    <t>212-555-7783</t>
+  </si>
+  <si>
+    <t>212-555-7784</t>
+  </si>
+  <si>
+    <t>212-555-7785</t>
+  </si>
+  <si>
+    <t>212-555-7786</t>
+  </si>
+  <si>
+    <t>212-555-7787</t>
+  </si>
+  <si>
+    <t>212-555-7788</t>
+  </si>
+  <si>
+    <t>212-555-7789</t>
+  </si>
+  <si>
+    <t>212-555-7790</t>
+  </si>
+  <si>
+    <t>212-555-7791</t>
+  </si>
+  <si>
+    <t>212-555-7792</t>
+  </si>
+  <si>
+    <t>212-555-7793</t>
+  </si>
+  <si>
+    <t>212-555-7794</t>
+  </si>
+  <si>
+    <t>212-555-7795</t>
+  </si>
+  <si>
+    <t>212-555-7796</t>
+  </si>
+  <si>
+    <t>212-555-7797</t>
+  </si>
+  <si>
+    <t>212-555-7798</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -912,6 +1011,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -934,7 +1045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -944,6 +1055,11 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1258,27 +1374,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52769B47-957A-4F9B-8A1C-849E74A1076A}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.40625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="7"/>
+    <col min="11" max="11" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1328125" customWidth="1"/>
+    <col min="14" max="14" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.86328125" customWidth="1"/>
+    <col min="16" max="16" width="15.953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1424,7 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -1316,13 +1437,28 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>291</v>
+      </c>
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="S1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1347,7 +1483,7 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="7">
         <v>12207</v>
       </c>
       <c r="J2" t="s">
@@ -1360,13 +1496,28 @@
         <v>99</v>
       </c>
       <c r="M2" t="s">
+        <v>292</v>
+      </c>
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>286</v>
+      </c>
+      <c r="P2" s="6">
+        <v>45407</v>
+      </c>
+      <c r="Q2">
+        <v>12345</v>
+      </c>
+      <c r="R2" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1391,7 +1542,7 @@
       <c r="H3" t="s">
         <v>102</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="7">
         <v>33101</v>
       </c>
       <c r="J3" t="s">
@@ -1404,13 +1555,28 @@
         <v>104</v>
       </c>
       <c r="M3" t="s">
+        <v>293</v>
+      </c>
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
+        <v>286</v>
+      </c>
+      <c r="P3" s="6">
+        <v>45408</v>
+      </c>
+      <c r="Q3">
+        <v>12346</v>
+      </c>
+      <c r="R3" t="s">
+        <v>288</v>
+      </c>
+      <c r="S3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1435,7 +1601,7 @@
       <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="7">
         <v>90001</v>
       </c>
       <c r="J4" t="s">
@@ -1448,13 +1614,28 @@
         <v>110</v>
       </c>
       <c r="M4" t="s">
+        <v>294</v>
+      </c>
+      <c r="N4" t="s">
         <v>16</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
+        <v>286</v>
+      </c>
+      <c r="P4" s="6">
+        <v>45409</v>
+      </c>
+      <c r="Q4">
+        <v>12347</v>
+      </c>
+      <c r="R4" t="s">
+        <v>289</v>
+      </c>
+      <c r="S4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -1479,7 +1660,7 @@
       <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="7">
         <v>90001</v>
       </c>
       <c r="J5" t="s">
@@ -1492,13 +1673,28 @@
         <v>114</v>
       </c>
       <c r="M5" t="s">
+        <v>295</v>
+      </c>
+      <c r="N5" t="s">
         <v>16</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
+        <v>286</v>
+      </c>
+      <c r="P5" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q5">
+        <v>12348</v>
+      </c>
+      <c r="R5" t="s">
+        <v>290</v>
+      </c>
+      <c r="S5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -1523,7 +1719,7 @@
       <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="7">
         <v>12207</v>
       </c>
       <c r="J6" t="s">
@@ -1536,13 +1732,28 @@
         <v>119</v>
       </c>
       <c r="M6" t="s">
+        <v>296</v>
+      </c>
+      <c r="N6" t="s">
         <v>16</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
+        <v>286</v>
+      </c>
+      <c r="P6" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q6">
+        <v>12349</v>
+      </c>
+      <c r="R6" t="s">
+        <v>287</v>
+      </c>
+      <c r="S6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -1567,7 +1778,7 @@
       <c r="H7" t="s">
         <v>102</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="7">
         <v>33101</v>
       </c>
       <c r="J7" t="s">
@@ -1580,13 +1791,28 @@
         <v>124</v>
       </c>
       <c r="M7" t="s">
+        <v>297</v>
+      </c>
+      <c r="N7" t="s">
         <v>16</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
+        <v>286</v>
+      </c>
+      <c r="P7" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q7">
+        <v>12350</v>
+      </c>
+      <c r="R7" t="s">
+        <v>288</v>
+      </c>
+      <c r="S7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -1611,7 +1837,7 @@
       <c r="H8" t="s">
         <v>19</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="7">
         <v>90001</v>
       </c>
       <c r="J8" t="s">
@@ -1624,13 +1850,28 @@
         <v>128</v>
       </c>
       <c r="M8" t="s">
+        <v>298</v>
+      </c>
+      <c r="N8" t="s">
         <v>16</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
+        <v>286</v>
+      </c>
+      <c r="P8" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q8">
+        <v>12351</v>
+      </c>
+      <c r="R8" t="s">
+        <v>289</v>
+      </c>
+      <c r="S8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -1655,7 +1896,7 @@
       <c r="H9" t="s">
         <v>19</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="7">
         <v>90001</v>
       </c>
       <c r="J9" t="s">
@@ -1668,13 +1909,28 @@
         <v>133</v>
       </c>
       <c r="M9" t="s">
+        <v>299</v>
+      </c>
+      <c r="N9" t="s">
         <v>16</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
+        <v>286</v>
+      </c>
+      <c r="P9" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q9">
+        <v>12352</v>
+      </c>
+      <c r="R9" t="s">
+        <v>290</v>
+      </c>
+      <c r="S9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -1699,7 +1955,7 @@
       <c r="H10" t="s">
         <v>14</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="7">
         <v>12207</v>
       </c>
       <c r="J10" t="s">
@@ -1712,13 +1968,28 @@
         <v>138</v>
       </c>
       <c r="M10" t="s">
+        <v>300</v>
+      </c>
+      <c r="N10" t="s">
         <v>16</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
+        <v>286</v>
+      </c>
+      <c r="P10" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q10">
+        <v>12353</v>
+      </c>
+      <c r="R10" t="s">
+        <v>287</v>
+      </c>
+      <c r="S10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -1743,7 +2014,7 @@
       <c r="H11" t="s">
         <v>102</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="7">
         <v>33101</v>
       </c>
       <c r="J11" t="s">
@@ -1756,13 +2027,28 @@
         <v>142</v>
       </c>
       <c r="M11" t="s">
+        <v>301</v>
+      </c>
+      <c r="N11" t="s">
         <v>16</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
+        <v>286</v>
+      </c>
+      <c r="P11" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q11">
+        <v>12354</v>
+      </c>
+      <c r="R11" t="s">
+        <v>288</v>
+      </c>
+      <c r="S11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -1787,7 +2073,7 @@
       <c r="H12" t="s">
         <v>19</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="7">
         <v>90001</v>
       </c>
       <c r="J12" t="s">
@@ -1800,13 +2086,28 @@
         <v>147</v>
       </c>
       <c r="M12" t="s">
+        <v>302</v>
+      </c>
+      <c r="N12" t="s">
         <v>16</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
+        <v>286</v>
+      </c>
+      <c r="P12" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q12">
+        <v>12355</v>
+      </c>
+      <c r="R12" t="s">
+        <v>289</v>
+      </c>
+      <c r="S12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -1831,7 +2132,7 @@
       <c r="H13" t="s">
         <v>19</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="7">
         <v>90001</v>
       </c>
       <c r="J13" t="s">
@@ -1844,13 +2145,28 @@
         <v>152</v>
       </c>
       <c r="M13" t="s">
+        <v>303</v>
+      </c>
+      <c r="N13" t="s">
         <v>16</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
+        <v>286</v>
+      </c>
+      <c r="P13" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q13">
+        <v>12356</v>
+      </c>
+      <c r="R13" t="s">
+        <v>290</v>
+      </c>
+      <c r="S13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1875,7 +2191,7 @@
       <c r="H14" t="s">
         <v>14</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="7">
         <v>12207</v>
       </c>
       <c r="J14" t="s">
@@ -1888,13 +2204,28 @@
         <v>156</v>
       </c>
       <c r="M14" t="s">
+        <v>304</v>
+      </c>
+      <c r="N14" t="s">
         <v>16</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
+        <v>286</v>
+      </c>
+      <c r="P14" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q14">
+        <v>12357</v>
+      </c>
+      <c r="R14" t="s">
+        <v>287</v>
+      </c>
+      <c r="S14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -1919,7 +2250,7 @@
       <c r="H15" t="s">
         <v>102</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="7">
         <v>33101</v>
       </c>
       <c r="J15" t="s">
@@ -1932,13 +2263,28 @@
         <v>160</v>
       </c>
       <c r="M15" t="s">
+        <v>305</v>
+      </c>
+      <c r="N15" t="s">
         <v>16</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
+        <v>286</v>
+      </c>
+      <c r="P15" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q15">
+        <v>12358</v>
+      </c>
+      <c r="R15" t="s">
+        <v>288</v>
+      </c>
+      <c r="S15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -1963,7 +2309,7 @@
       <c r="H16" t="s">
         <v>19</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="7">
         <v>90001</v>
       </c>
       <c r="J16" t="s">
@@ -1976,13 +2322,28 @@
         <v>165</v>
       </c>
       <c r="M16" t="s">
+        <v>306</v>
+      </c>
+      <c r="N16" t="s">
         <v>16</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
+        <v>286</v>
+      </c>
+      <c r="P16" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q16">
+        <v>12359</v>
+      </c>
+      <c r="R16" t="s">
+        <v>289</v>
+      </c>
+      <c r="S16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -2007,7 +2368,7 @@
       <c r="H17" t="s">
         <v>14</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="7">
         <v>12207</v>
       </c>
       <c r="J17" t="s">
@@ -2020,13 +2381,28 @@
         <v>170</v>
       </c>
       <c r="M17" t="s">
+        <v>307</v>
+      </c>
+      <c r="N17" t="s">
         <v>16</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
+        <v>286</v>
+      </c>
+      <c r="P17" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q17">
+        <v>12360</v>
+      </c>
+      <c r="R17" t="s">
+        <v>290</v>
+      </c>
+      <c r="S17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -2051,7 +2427,7 @@
       <c r="H18" t="s">
         <v>102</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="7">
         <v>33101</v>
       </c>
       <c r="J18" t="s">
@@ -2064,13 +2440,28 @@
         <v>174</v>
       </c>
       <c r="M18" t="s">
+        <v>308</v>
+      </c>
+      <c r="N18" t="s">
         <v>16</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
+        <v>286</v>
+      </c>
+      <c r="P18" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q18">
+        <v>12361</v>
+      </c>
+      <c r="R18" t="s">
+        <v>287</v>
+      </c>
+      <c r="S18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>175</v>
       </c>
@@ -2095,7 +2486,7 @@
       <c r="H19" t="s">
         <v>19</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="7">
         <v>90001</v>
       </c>
       <c r="J19" t="s">
@@ -2108,13 +2499,28 @@
         <v>179</v>
       </c>
       <c r="M19" t="s">
+        <v>309</v>
+      </c>
+      <c r="N19" t="s">
         <v>16</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
+        <v>286</v>
+      </c>
+      <c r="P19" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q19">
+        <v>12362</v>
+      </c>
+      <c r="R19" t="s">
+        <v>288</v>
+      </c>
+      <c r="S19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -2139,7 +2545,7 @@
       <c r="H20" t="s">
         <v>19</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="7">
         <v>90001</v>
       </c>
       <c r="J20" t="s">
@@ -2152,13 +2558,28 @@
         <v>179</v>
       </c>
       <c r="M20" t="s">
+        <v>310</v>
+      </c>
+      <c r="N20" t="s">
         <v>16</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P20" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q20">
+        <v>12363</v>
+      </c>
+      <c r="R20" t="s">
+        <v>289</v>
+      </c>
+      <c r="S20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>182</v>
       </c>
@@ -2183,7 +2604,7 @@
       <c r="H21" t="s">
         <v>14</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="7">
         <v>12207</v>
       </c>
       <c r="J21" t="s">
@@ -2196,13 +2617,28 @@
         <v>188</v>
       </c>
       <c r="M21" t="s">
+        <v>311</v>
+      </c>
+      <c r="N21" t="s">
         <v>16</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
+        <v>286</v>
+      </c>
+      <c r="P21" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q21">
+        <v>12364</v>
+      </c>
+      <c r="R21" t="s">
+        <v>290</v>
+      </c>
+      <c r="S21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>189</v>
       </c>
@@ -2227,7 +2663,7 @@
       <c r="H22" t="s">
         <v>102</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="7">
         <v>33101</v>
       </c>
       <c r="J22" t="s">
@@ -2240,13 +2676,28 @@
         <v>193</v>
       </c>
       <c r="M22" t="s">
+        <v>312</v>
+      </c>
+      <c r="N22" t="s">
         <v>16</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
+        <v>286</v>
+      </c>
+      <c r="P22" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q22">
+        <v>12365</v>
+      </c>
+      <c r="R22" t="s">
+        <v>287</v>
+      </c>
+      <c r="S22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>194</v>
       </c>
@@ -2271,7 +2722,7 @@
       <c r="H23" t="s">
         <v>14</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="7">
         <v>12207</v>
       </c>
       <c r="J23" t="s">
@@ -2284,14 +2735,31 @@
         <v>198</v>
       </c>
       <c r="M23" t="s">
+        <v>313</v>
+      </c>
+      <c r="N23" t="s">
         <v>16</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
+        <v>286</v>
+      </c>
+      <c r="P23" s="6">
+        <v>45410</v>
+      </c>
+      <c r="Q23">
+        <v>12366</v>
+      </c>
+      <c r="R23" t="s">
+        <v>288</v>
+      </c>
+      <c r="S23" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2299,21 +2767,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6396F3-6D7B-46A0-9EAC-B306C37237B1}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2333,7 +2801,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2350,7 +2818,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2367,7 +2835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2384,7 +2852,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2401,7 +2869,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2418,7 +2886,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -2432,7 +2900,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -2446,7 +2914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2460,7 +2928,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2477,7 +2945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2494,7 +2962,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2511,7 +2979,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2528,7 +2996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2542,7 +3010,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2559,7 +3027,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -2576,7 +3044,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -2593,7 +3061,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2610,7 +3078,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2627,7 +3095,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -2644,7 +3112,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -2674,15 +3142,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.40625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2696,7 +3164,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2710,7 +3178,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2724,7 +3192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2738,7 +3206,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -2752,7 +3220,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -2779,19 +3247,19 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>220</v>
       </c>
@@ -2820,7 +3288,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>224</v>
       </c>
@@ -2849,7 +3317,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -2878,7 +3346,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>253</v>
       </c>
@@ -2907,7 +3375,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>261</v>
       </c>
@@ -2949,17 +3417,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.40625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>228</v>
       </c>
@@ -2979,7 +3447,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>243</v>
       </c>
@@ -2999,7 +3467,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>235</v>
       </c>
@@ -3019,7 +3487,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>238</v>
       </c>
@@ -3039,7 +3507,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>241</v>
       </c>

</xml_diff>